<commit_message>
removing the result column
</commit_message>
<xml_diff>
--- a/Workbook2.xlsx
+++ b/Workbook2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25620" windowHeight="16240" tabRatio="500" activeTab="1"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="25620" windowHeight="16240" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="189">
   <si>
     <t>userID</t>
   </si>
@@ -581,6 +581,12 @@
   </si>
   <si>
     <t>soup</t>
+  </si>
+  <si>
+    <t>img</t>
+  </si>
+  <si>
+    <t>Unique</t>
   </si>
 </sst>
 </file>
@@ -663,7 +669,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -723,6 +729,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="123">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -849,7 +900,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -885,6 +936,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -894,22 +951,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1892,10 +1940,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O40"/>
+  <dimension ref="A1:P40"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1911,37 +1959,36 @@
     <col min="10" max="10" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13.6640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="13.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="16" thickBot="1">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:15" ht="16" thickBot="1">
+      <c r="A1" s="19" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="19"/>
-    </row>
-    <row r="2" spans="1:14">
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="20"/>
+      <c r="I1" s="20"/>
+      <c r="J1" s="20"/>
+      <c r="K1" s="20"/>
+      <c r="L1" s="20"/>
+      <c r="M1" s="20"/>
+      <c r="N1" s="20"/>
+      <c r="O1" s="21"/>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="12" t="s">
         <v>171</v>
       </c>
       <c r="B2" s="12" t="s">
         <v>172</v>
       </c>
-      <c r="C2" s="12" t="s">
-        <v>172</v>
-      </c>
+      <c r="C2" s="12"/>
       <c r="D2" s="16"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
@@ -1952,13 +1999,14 @@
       <c r="K2" s="12"/>
       <c r="L2" s="12"/>
       <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-    </row>
-    <row r="3" spans="1:14" ht="16">
+      <c r="N2" s="16"/>
+      <c r="O2" s="12"/>
+    </row>
+    <row r="3" spans="1:15" ht="16">
       <c r="A3" s="15" t="s">
         <v>164</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="14" t="s">
@@ -1994,19 +2042,22 @@
       <c r="M3" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="N3" s="13" t="s">
+        <v>187</v>
+      </c>
+      <c r="O3" s="14" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="4" spans="1:14">
+    <row r="4" spans="1:15">
       <c r="A4" s="15">
         <v>1</v>
       </c>
-      <c r="B4" s="24">
+      <c r="B4" s="18">
         <v>123</v>
       </c>
-      <c r="C4" s="14">
-        <v>534534534</v>
+      <c r="C4" s="14" t="s">
+        <v>188</v>
       </c>
       <c r="D4" s="8" t="s">
         <v>185</v>
@@ -2038,19 +2089,20 @@
       <c r="M4" s="8" t="b">
         <v>1</v>
       </c>
-      <c r="N4" s="8" t="b">
+      <c r="N4" s="8"/>
+      <c r="O4" s="8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:14">
+    <row r="5" spans="1:15">
       <c r="A5" s="15">
         <v>2</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="18">
         <v>123</v>
       </c>
-      <c r="C5" s="14">
-        <v>534534535</v>
+      <c r="C5" s="14" t="s">
+        <v>188</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>186</v>
@@ -2082,18 +2134,21 @@
       <c r="M5" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="N5" s="8" t="b">
+      <c r="N5" s="8"/>
+      <c r="O5" s="8" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:14">
+    <row r="6" spans="1:15">
       <c r="A6" s="15">
         <v>3</v>
       </c>
-      <c r="B6" s="24">
+      <c r="B6" s="18">
         <v>123</v>
       </c>
-      <c r="C6" s="14"/>
+      <c r="C6" s="14" t="s">
+        <v>188</v>
+      </c>
       <c r="D6" s="8"/>
       <c r="E6" s="8"/>
       <c r="F6" s="8"/>
@@ -2105,15 +2160,18 @@
       <c r="L6" s="8"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="O6" s="8"/>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="15">
         <v>4</v>
       </c>
-      <c r="B7" s="24">
+      <c r="B7" s="18">
         <v>123</v>
       </c>
-      <c r="C7" s="14"/>
+      <c r="C7" s="14" t="s">
+        <v>188</v>
+      </c>
       <c r="D7" s="8"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -2125,15 +2183,18 @@
       <c r="L7" s="8"/>
       <c r="M7" s="8"/>
       <c r="N7" s="8"/>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="O7" s="8"/>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="15">
         <v>5</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="18">
         <v>123</v>
       </c>
-      <c r="C8" s="14"/>
+      <c r="C8" s="14" t="s">
+        <v>188</v>
+      </c>
       <c r="D8" s="8"/>
       <c r="E8" s="8"/>
       <c r="F8" s="8"/>
@@ -2145,15 +2206,18 @@
       <c r="L8" s="8"/>
       <c r="M8" s="8"/>
       <c r="N8" s="8"/>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="O8" s="8"/>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="15">
         <v>6</v>
       </c>
-      <c r="B9" s="24">
+      <c r="B9" s="18">
         <v>123</v>
       </c>
-      <c r="C9" s="14"/>
+      <c r="C9" s="14" t="s">
+        <v>188</v>
+      </c>
       <c r="D9" s="8"/>
       <c r="E9" s="8"/>
       <c r="F9" s="8"/>
@@ -2165,15 +2229,18 @@
       <c r="L9" s="8"/>
       <c r="M9" s="8"/>
       <c r="N9" s="8"/>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="O9" s="8"/>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="15">
         <v>7</v>
       </c>
-      <c r="B10" s="24">
+      <c r="B10" s="18">
         <v>123</v>
       </c>
-      <c r="C10" s="14"/>
+      <c r="C10" s="14" t="s">
+        <v>188</v>
+      </c>
       <c r="D10" s="8"/>
       <c r="E10" s="8"/>
       <c r="F10" s="8"/>
@@ -2185,15 +2252,18 @@
       <c r="L10" s="8"/>
       <c r="M10" s="8"/>
       <c r="N10" s="8"/>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="O10" s="8"/>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="15">
         <v>8</v>
       </c>
-      <c r="B11" s="24">
+      <c r="B11" s="18">
         <v>123</v>
       </c>
-      <c r="C11" s="14"/>
+      <c r="C11" s="14" t="s">
+        <v>188</v>
+      </c>
       <c r="D11" s="8"/>
       <c r="E11" s="8"/>
       <c r="F11" s="8"/>
@@ -2205,15 +2275,18 @@
       <c r="L11" s="8"/>
       <c r="M11" s="8"/>
       <c r="N11" s="8"/>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="O11" s="8"/>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="15">
         <v>9</v>
       </c>
-      <c r="B12" s="24">
+      <c r="B12" s="18">
         <v>123</v>
       </c>
-      <c r="C12" s="14"/>
+      <c r="C12" s="14" t="s">
+        <v>188</v>
+      </c>
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
@@ -2225,15 +2298,18 @@
       <c r="L12" s="8"/>
       <c r="M12" s="8"/>
       <c r="N12" s="8"/>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="O12" s="8"/>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="15">
         <v>10</v>
       </c>
-      <c r="B13" s="24">
+      <c r="B13" s="18">
         <v>123</v>
       </c>
-      <c r="C13" s="14"/>
+      <c r="C13" s="14" t="s">
+        <v>188</v>
+      </c>
       <c r="D13" s="8"/>
       <c r="E13" s="8"/>
       <c r="F13" s="8"/>
@@ -2245,15 +2321,18 @@
       <c r="L13" s="8"/>
       <c r="M13" s="8"/>
       <c r="N13" s="8"/>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="O13" s="8"/>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="15">
         <v>11</v>
       </c>
-      <c r="B14" s="24">
+      <c r="B14" s="18">
         <v>123</v>
       </c>
-      <c r="C14" s="14"/>
+      <c r="C14" s="14" t="s">
+        <v>188</v>
+      </c>
       <c r="D14" s="8"/>
       <c r="E14" s="8"/>
       <c r="F14" s="8"/>
@@ -2265,15 +2344,18 @@
       <c r="L14" s="8"/>
       <c r="M14" s="8"/>
       <c r="N14" s="8"/>
-    </row>
-    <row r="15" spans="1:14">
+      <c r="O14" s="8"/>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="15">
         <v>12</v>
       </c>
-      <c r="B15" s="24">
+      <c r="B15" s="18">
         <v>123</v>
       </c>
-      <c r="C15" s="14"/>
+      <c r="C15" s="14" t="s">
+        <v>188</v>
+      </c>
       <c r="D15" s="8"/>
       <c r="E15" s="8"/>
       <c r="F15" s="8"/>
@@ -2285,15 +2367,18 @@
       <c r="L15" s="8"/>
       <c r="M15" s="8"/>
       <c r="N15" s="8"/>
-    </row>
-    <row r="16" spans="1:14">
+      <c r="O15" s="8"/>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="15">
         <v>13</v>
       </c>
-      <c r="B16" s="24">
+      <c r="B16" s="18">
         <v>123</v>
       </c>
-      <c r="C16" s="14"/>
+      <c r="C16" s="14" t="s">
+        <v>188</v>
+      </c>
       <c r="D16" s="8"/>
       <c r="E16" s="8"/>
       <c r="F16" s="8"/>
@@ -2305,15 +2390,18 @@
       <c r="L16" s="8"/>
       <c r="M16" s="8"/>
       <c r="N16" s="8"/>
-    </row>
-    <row r="17" spans="1:15">
+      <c r="O16" s="8"/>
+    </row>
+    <row r="17" spans="1:16">
       <c r="A17" s="15">
         <v>14</v>
       </c>
-      <c r="B17" s="24">
+      <c r="B17" s="18">
         <v>123</v>
       </c>
-      <c r="C17" s="25"/>
+      <c r="C17" s="14" t="s">
+        <v>188</v>
+      </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
@@ -2325,8 +2413,9 @@
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
       <c r="N17" s="15"/>
-    </row>
-    <row r="18" spans="1:15" ht="16" thickBot="1">
+      <c r="O17" s="15"/>
+    </row>
+    <row r="18" spans="1:16" ht="16" thickBot="1">
       <c r="A18" s="12"/>
       <c r="B18" s="12"/>
       <c r="C18" s="12"/>
@@ -2340,27 +2429,28 @@
       <c r="K18" s="12"/>
       <c r="L18" s="12"/>
       <c r="M18" s="12"/>
-      <c r="N18" s="12"/>
-    </row>
-    <row r="19" spans="1:15" ht="16" thickBot="1">
+      <c r="N18" s="16"/>
+      <c r="O18" s="12"/>
+    </row>
+    <row r="19" spans="1:16" ht="16" thickBot="1">
       <c r="A19" s="12"/>
-      <c r="B19" s="20" t="s">
+      <c r="B19" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="22"/>
-      <c r="M19" s="12"/>
+      <c r="C19" s="23"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
+      <c r="F19" s="23"/>
+      <c r="G19" s="23"/>
+      <c r="H19" s="23"/>
+      <c r="I19" s="23"/>
+      <c r="J19" s="23"/>
+      <c r="K19" s="24"/>
+      <c r="L19" s="12"/>
+      <c r="M19" s="16"/>
       <c r="N19" s="12"/>
     </row>
-    <row r="20" spans="1:15">
+    <row r="20" spans="1:16">
       <c r="A20" s="12"/>
       <c r="B20" s="12" t="s">
         <v>171</v>
@@ -2376,53 +2466,55 @@
       <c r="K20" s="12"/>
       <c r="L20" s="12"/>
       <c r="M20" s="12"/>
-      <c r="N20" s="12"/>
-    </row>
-    <row r="21" spans="1:15" ht="16">
+      <c r="N20" s="16"/>
+      <c r="O20" s="12"/>
+    </row>
+    <row r="21" spans="1:16" ht="16">
       <c r="A21" s="12"/>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="17" t="s">
         <v>162</v>
       </c>
       <c r="C21" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="D21" s="13"/>
-      <c r="E21" s="14" t="s">
+      <c r="D21" s="14" t="s">
         <v>177</v>
       </c>
+      <c r="E21" s="11" t="s">
+        <v>178</v>
+      </c>
       <c r="F21" s="11" t="s">
-        <v>178</v>
-      </c>
-      <c r="G21" s="11" t="s">
         <v>179</v>
       </c>
+      <c r="G21" s="13" t="s">
+        <v>180</v>
+      </c>
       <c r="H21" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="I21" s="13" t="s">
         <v>181</v>
       </c>
+      <c r="I21" s="14" t="s">
+        <v>182</v>
+      </c>
       <c r="J21" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="K21" s="14" t="s">
         <v>183</v>
       </c>
-      <c r="L21" s="13" t="s">
+      <c r="K21" s="13" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="22" spans="1:15">
+    <row r="22" spans="1:16">
       <c r="A22" s="12"/>
-      <c r="B22" s="23">
+      <c r="B22" s="17">
         <v>123</v>
       </c>
       <c r="C22" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="D22" s="9"/>
+      <c r="D22" s="9" t="b">
+        <v>1</v>
+      </c>
       <c r="E22" s="9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F22" s="9" t="b">
         <v>0</v>
@@ -2442,11 +2534,8 @@
       <c r="K22" s="9" t="b">
         <v>0</v>
       </c>
-      <c r="L22" s="9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15">
+    </row>
+    <row r="23" spans="1:16">
       <c r="A23" s="12"/>
       <c r="B23" s="10"/>
       <c r="C23" s="10"/>
@@ -2460,8 +2549,9 @@
       <c r="K23" s="10"/>
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
-    </row>
-    <row r="24" spans="1:15">
+      <c r="N23" s="16"/>
+    </row>
+    <row r="24" spans="1:16">
       <c r="A24" s="12"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10"/>
@@ -2475,8 +2565,9 @@
       <c r="K24" s="10"/>
       <c r="L24" s="12"/>
       <c r="M24" s="12"/>
-    </row>
-    <row r="25" spans="1:15">
+      <c r="N24" s="16"/>
+    </row>
+    <row r="25" spans="1:16">
       <c r="A25" s="12"/>
       <c r="B25" s="12"/>
       <c r="C25" s="12"/>
@@ -2488,8 +2579,9 @@
       <c r="K25" s="12"/>
       <c r="L25" s="12"/>
       <c r="M25" s="12"/>
-    </row>
-    <row r="26" spans="1:15">
+      <c r="N25" s="16"/>
+    </row>
+    <row r="26" spans="1:16">
       <c r="A26" s="12"/>
       <c r="B26" s="12"/>
       <c r="C26" s="12"/>
@@ -2501,9 +2593,10 @@
       <c r="K26" s="12"/>
       <c r="L26" s="12"/>
       <c r="M26" s="12"/>
-      <c r="N26" s="12"/>
-    </row>
-    <row r="27" spans="1:15">
+      <c r="N26" s="16"/>
+      <c r="O26" s="12"/>
+    </row>
+    <row r="27" spans="1:16">
       <c r="A27" s="12"/>
       <c r="B27" s="12"/>
       <c r="C27" s="12"/>
@@ -2515,9 +2608,10 @@
       <c r="K27" s="12"/>
       <c r="L27" s="12"/>
       <c r="M27" s="12"/>
-      <c r="N27" s="12"/>
-    </row>
-    <row r="28" spans="1:15">
+      <c r="N27" s="16"/>
+      <c r="O27" s="12"/>
+    </row>
+    <row r="28" spans="1:16">
       <c r="A28" s="12"/>
       <c r="B28" s="12"/>
       <c r="C28" s="12"/>
@@ -2529,9 +2623,10 @@
       <c r="K28" s="12"/>
       <c r="L28" s="12"/>
       <c r="M28" s="12"/>
-      <c r="N28" s="12"/>
-    </row>
-    <row r="29" spans="1:15">
+      <c r="N28" s="16"/>
+      <c r="O28" s="12"/>
+    </row>
+    <row r="29" spans="1:16">
       <c r="A29" s="12"/>
       <c r="B29" s="12"/>
       <c r="C29" s="12"/>
@@ -2543,10 +2638,11 @@
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
       <c r="M29" s="12"/>
-      <c r="N29" s="12"/>
+      <c r="N29" s="16"/>
       <c r="O29" s="12"/>
-    </row>
-    <row r="30" spans="1:15">
+      <c r="P29" s="12"/>
+    </row>
+    <row r="30" spans="1:16">
       <c r="A30" s="12"/>
       <c r="B30" s="12"/>
       <c r="C30" s="12"/>
@@ -2558,10 +2654,11 @@
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
       <c r="M30" s="12"/>
-      <c r="N30" s="12"/>
+      <c r="N30" s="16"/>
       <c r="O30" s="12"/>
-    </row>
-    <row r="31" spans="1:15">
+      <c r="P30" s="12"/>
+    </row>
+    <row r="31" spans="1:16">
       <c r="A31" s="12"/>
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
@@ -2573,10 +2670,11 @@
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
       <c r="M31" s="12"/>
-      <c r="N31" s="12"/>
+      <c r="N31" s="16"/>
       <c r="O31" s="12"/>
-    </row>
-    <row r="32" spans="1:15">
+      <c r="P31" s="12"/>
+    </row>
+    <row r="32" spans="1:16">
       <c r="A32" s="12"/>
       <c r="B32" s="12"/>
       <c r="C32" s="12"/>
@@ -2588,10 +2686,11 @@
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
       <c r="M32" s="12"/>
-      <c r="N32" s="12"/>
+      <c r="N32" s="16"/>
       <c r="O32" s="12"/>
-    </row>
-    <row r="33" spans="1:15">
+      <c r="P32" s="12"/>
+    </row>
+    <row r="33" spans="1:16">
       <c r="A33" s="12"/>
       <c r="B33" s="12"/>
       <c r="C33" s="12"/>
@@ -2603,10 +2702,11 @@
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
       <c r="M33" s="12"/>
-      <c r="N33" s="12"/>
+      <c r="N33" s="16"/>
       <c r="O33" s="12"/>
-    </row>
-    <row r="34" spans="1:15">
+      <c r="P33" s="12"/>
+    </row>
+    <row r="34" spans="1:16">
       <c r="A34" s="12"/>
       <c r="B34" s="12"/>
       <c r="C34" s="12"/>
@@ -2618,10 +2718,11 @@
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
       <c r="M34" s="12"/>
-      <c r="N34" s="12"/>
+      <c r="N34" s="16"/>
       <c r="O34" s="12"/>
-    </row>
-    <row r="35" spans="1:15">
+      <c r="P34" s="12"/>
+    </row>
+    <row r="35" spans="1:16">
       <c r="A35" s="12"/>
       <c r="B35" s="12"/>
       <c r="C35" s="12"/>
@@ -2633,10 +2734,11 @@
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
       <c r="M35" s="12"/>
-      <c r="N35" s="12"/>
+      <c r="N35" s="16"/>
       <c r="O35" s="12"/>
-    </row>
-    <row r="36" spans="1:15">
+      <c r="P35" s="12"/>
+    </row>
+    <row r="36" spans="1:16">
       <c r="A36" s="12"/>
       <c r="B36" s="12"/>
       <c r="C36" s="12"/>
@@ -2648,10 +2750,11 @@
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
       <c r="M36" s="12"/>
-      <c r="N36" s="12"/>
+      <c r="N36" s="16"/>
       <c r="O36" s="12"/>
-    </row>
-    <row r="37" spans="1:15">
+      <c r="P36" s="12"/>
+    </row>
+    <row r="37" spans="1:16">
       <c r="A37" s="12"/>
       <c r="B37" s="12"/>
       <c r="C37" s="12"/>
@@ -2663,10 +2766,11 @@
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
       <c r="M37" s="12"/>
-      <c r="N37" s="12"/>
+      <c r="N37" s="16"/>
       <c r="O37" s="12"/>
-    </row>
-    <row r="38" spans="1:15">
+      <c r="P37" s="12"/>
+    </row>
+    <row r="38" spans="1:16">
       <c r="A38" s="12"/>
       <c r="B38" s="12"/>
       <c r="C38" s="12"/>
@@ -2678,10 +2782,11 @@
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
       <c r="M38" s="12"/>
-      <c r="N38" s="12"/>
+      <c r="N38" s="16"/>
       <c r="O38" s="12"/>
-    </row>
-    <row r="39" spans="1:15">
+      <c r="P38" s="12"/>
+    </row>
+    <row r="39" spans="1:16">
       <c r="A39" s="12"/>
       <c r="B39" s="12"/>
       <c r="C39" s="12"/>
@@ -2693,10 +2798,11 @@
       <c r="K39" s="12"/>
       <c r="L39" s="12"/>
       <c r="M39" s="12"/>
-      <c r="N39" s="12"/>
+      <c r="N39" s="16"/>
       <c r="O39" s="12"/>
-    </row>
-    <row r="40" spans="1:15">
+      <c r="P39" s="12"/>
+    </row>
+    <row r="40" spans="1:16">
       <c r="A40" s="12"/>
       <c r="B40" s="12"/>
       <c r="C40" s="12"/>
@@ -2708,13 +2814,14 @@
       <c r="K40" s="12"/>
       <c r="L40" s="12"/>
       <c r="M40" s="12"/>
-      <c r="N40" s="12"/>
+      <c r="N40" s="16"/>
       <c r="O40" s="12"/>
+      <c r="P40" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:N1"/>
-    <mergeCell ref="B19:L19"/>
+    <mergeCell ref="A1:O1"/>
+    <mergeCell ref="B19:K19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>